<commit_message>
the multiple data provider is in progress
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginTest.xlsx
+++ b/src/test/resources/LoginTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechTeam-08\IdeaProjects\tutorial_project_for_automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6DB2F6-21C9-48ED-9DBB-D8DE647090F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D497D2EB-5879-4928-A515-786F3737F3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>username</t>
   </si>
@@ -61,6 +61,42 @@
   </si>
   <si>
     <t>haha</t>
+  </si>
+  <si>
+    <t>fart</t>
+  </si>
+  <si>
+    <t>dumb</t>
+  </si>
+  <si>
+    <t>agree</t>
+  </si>
+  <si>
+    <t>nah</t>
+  </si>
+  <si>
+    <t>lol</t>
+  </si>
+  <si>
+    <t>yoo</t>
+  </si>
+  <si>
+    <t>damn</t>
+  </si>
+  <si>
+    <t>gari</t>
+  </si>
+  <si>
+    <t>chole na</t>
+  </si>
+  <si>
+    <t>kiu</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>lalalalal</t>
   </si>
 </sst>
 </file>
@@ -378,15 +414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -396,8 +432,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -407,8 +449,14 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -418,8 +466,14 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -428,6 +482,29 @@
       </c>
       <c r="C4" t="s">
         <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>